<commit_message>
feat: Add BGM of MainMenu resource files
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/Groovy/res/sound/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres 복사본/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617E9328-6345-5449-9D49-867422902116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E467432-3069-DC4F-9C42-201410B0C21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27180" yWindow="-8560" windowWidth="19200" windowHeight="21100" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
@@ -36,12 +36,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>S</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,6 +78,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TitleScreen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Audio Normalization</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,6 +94,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>AlienSpaceship.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceHanger.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AmbientSpace.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>SpaceInvadersOST_Earth.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -110,11 +134,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>MainMenu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Level5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SpaceInvadersOST_Jupiter.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spacedrone.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -527,45 +559,45 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G16" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
@@ -574,22 +606,22 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -598,22 +630,22 @@
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -622,22 +654,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -646,22 +678,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -670,22 +702,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -694,26 +726,122 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>BGM_LevelDesign_GameScreen_Level7_SpaceInvaders OST_Saturn.wav</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>BGM_MainMenu_TitleScreen_Main_Spacedrone.wav</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_LevelDesign_GameScreen_Level7_SpaceInvaders OST_Saturn.wav</v>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>BGM_MainMenu_TitleScreen_Main_AlienSpaceship.wav</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>BGM_MainMenu_TitleScreen_Main_SpaceHanger.wav</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>BGM_MainMenu_TitleScreen_Main_AmbientSpace.wav</v>
       </c>
     </row>
     <row r="13" spans="1:7">

</xml_diff>

<commit_message>
feat: Add SFX of MainMenu resource file
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres 복사본/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/Groovy/res/sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E467432-3069-DC4F-9C42-201410B0C21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DD154D-0576-BE4C-BD58-5DA46502B6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27180" yWindow="-8560" windowWidth="19200" windowHeight="21100" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
+    <workbookView xWindow="-27180" yWindow="-8560" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
   <sheets>
     <sheet name="BGM" sheetId="1" r:id="rId1"/>
+    <sheet name="SFX" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,6 +85,13 @@
   <si>
     <t>TitleScreen</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MenuSelect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlipLow.wav</t>
   </si>
   <si>
     <t>Audio Normalization</t>
@@ -544,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AD9B3-E95F-7D4D-82EC-7C2F601D1C79}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="220" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -559,30 +567,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -591,22 +599,22 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G16" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <f t="shared" ref="G2:G12" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
         <v>BGM_LevelDesign_GameScreen_Level1_SpaceInvadersOST_Venus.wav</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -615,13 +623,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -630,7 +638,7 @@
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -639,13 +647,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -654,7 +662,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -663,13 +671,13 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -678,22 +686,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -702,7 +710,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -711,13 +719,13 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -726,7 +734,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -735,13 +743,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -750,7 +758,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -759,13 +767,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -774,7 +782,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -783,13 +791,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -798,7 +806,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -807,13 +815,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -822,7 +830,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -831,13 +839,13 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -859,4 +867,79 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE52464-EF18-2641-8F7C-C87CF4B5A50E}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="154" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <v>SFX_MainMenu_TitleScreen_MenuSelect_BlipLow.wav</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
+    <sortCondition ref="G2:G20"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add SFX of Game Start & End resource file
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/Groovy/res/sound/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres 복사본/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DD154D-0576-BE4C-BD58-5DA46502B6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D10C730-8EFC-C74B-98FB-D55A56F4A8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27180" yWindow="-8560" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,6 +87,28 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>GameOver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AscendingScales2.wav</t>
+  </si>
+  <si>
+    <t>DescendingScales2.wav</t>
+  </si>
+  <si>
+    <t>LevelClear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LevelStartCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LevelStartBeep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>MenuSelect</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -94,6 +116,12 @@
     <t>BlipLow.wav</t>
   </si>
   <si>
+    <t>BlipHiShort.wav</t>
+  </si>
+  <si>
+    <t>BlipHiLong.wav</t>
+  </si>
+  <si>
     <t>Audio Normalization</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -147,6 +175,10 @@
   </si>
   <si>
     <t>Level5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameplayHUD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -567,30 +599,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -599,22 +631,22 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G12" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <f t="shared" ref="G2:G16" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
         <v>BGM_LevelDesign_GameScreen_Level1_SpaceInvadersOST_Venus.wav</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -623,13 +655,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -638,7 +670,7 @@
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -647,13 +679,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -662,7 +694,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -671,13 +703,13 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -686,22 +718,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -710,7 +742,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -719,13 +751,13 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -734,7 +766,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -743,13 +775,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -758,7 +790,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -767,13 +799,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -782,7 +814,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -791,13 +823,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -806,7 +838,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -815,13 +847,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -830,7 +862,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -839,13 +871,13 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -887,48 +919,144 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G5" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <v>SFX_GameplayHUD_GameScreen_GameOver_DescendingScales2.wav</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_GameplayHUD_GameScreen_LevelClear_AscendingScales2.wav</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_GameplayHUD_GameScreen_LevelStartBeep_BlipHiLong.wav</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_GameplayHUD_GameScreen_LevelStartCount_BlipHiShort.wav</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="str">
+        <f>_xlfn.CONCAT("SFX_",A6,"_",B6,"_",C6,"_",D6)</f>
         <v>SFX_MainMenu_TitleScreen_MenuSelect_BlipLow.wav</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add SFX of Ship and Bullet resource file
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres 복사본/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D10C730-8EFC-C74B-98FB-D55A56F4A8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA28B87D-0B47-9D45-8CA3-8CAE03BA31D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27180" yWindow="-8560" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,6 +97,21 @@
     <t>DescendingScales2.wav</t>
   </si>
   <si>
+    <t>DescendingScales1.wav</t>
+  </si>
+  <si>
+    <t>EnemyShipSpecial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyShipSpecialDestroy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllyShipDestroy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>LevelClear</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -113,15 +128,57 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ExplosionShort.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllyShipShooting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>BlipLow.wav</t>
   </si>
   <si>
+    <t>ExplosionLong.wav</t>
+  </si>
+  <si>
+    <t>EnemyShipDestroy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deleted.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>BlipHiShort.wav</t>
   </si>
   <si>
     <t>BlipHiLong.wav</t>
   </si>
   <si>
+    <t>EnemyShipShooting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LaserShootEnemy1.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LaserShootAlly1.wav</t>
+  </si>
+  <si>
+    <t>Bullet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyShip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Audio Normalization</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -174,11 +231,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Player&amp;EnemyShipVariety</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Level5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>AllyShipDestroyLives</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>GameplayHUD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShipAppear.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -599,30 +668,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -631,13 +700,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G16" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
@@ -646,7 +715,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -655,13 +724,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -670,7 +739,7 @@
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -679,13 +748,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -694,7 +763,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -703,13 +772,13 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -718,22 +787,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -742,7 +811,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -751,13 +820,13 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -766,7 +835,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -775,13 +844,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -790,7 +859,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -799,13 +868,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -814,7 +883,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -823,13 +892,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -838,7 +907,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -847,13 +916,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -862,7 +931,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -871,13 +940,13 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -903,7 +972,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE52464-EF18-2641-8F7C-C87CF4B5A50E}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="154" workbookViewId="0"/>
   </sheetViews>
@@ -919,30 +988,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -957,22 +1026,22 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G5" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <f t="shared" ref="G2:G20" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
         <v>SFX_GameplayHUD_GameScreen_GameOver_DescendingScales2.wav</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -981,7 +1050,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -990,22 +1059,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -1014,22 +1083,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -1038,30 +1107,195 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G6" t="str">
         <f>_xlfn.CONCAT("SFX_",A6,"_",B6,"_",C6,"_",D6)</f>
         <v>SFX_MainMenu_TitleScreen_MenuSelect_BlipLow.wav</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="1"/>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="str">
+        <f>_xlfn.CONCAT("SFX_",A7,"_",B7,"_",C7,"_",D7)</f>
+        <v>SFX_Player&amp;EnemyShipVariety_Bullet_AllyShipShooting_LaserShootAlly1.wav</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="str">
+        <f>_xlfn.CONCAT("SFX_",A8,"_",B8,"_",C8,"_",D8)</f>
+        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipDestroy_Deleted.wav</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="str">
+        <f>_xlfn.CONCAT("SFX_",A9,"_",B9,"_",C9,"_",D9)</f>
+        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipShooting_LaserShootEnemy1.wav</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="str">
+        <f>_xlfn.CONCAT("SFX_",A10,"_",B10,"_",C10,"_",D10)</f>
+        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipSpecial_ShipAppear.wav</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="str">
+        <f>_xlfn.CONCAT("SFX_",A11,"_",B11,"_",C11,"_",D11)</f>
+        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipSpecialDestroy_ExplosionShort.wav</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="str">
+        <f>_xlfn.CONCAT("SFX_",A12,"_",B12,"_",C12,"_",D12)</f>
+        <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroy_ExplosionLong.wav</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="str">
+        <f>_xlfn.CONCAT("SFX_",A13,"_",B13,"_",C13,"_",D13)</f>
+        <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroyLives_DescendingScales1.wav</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">

</xml_diff>

<commit_message>
feat: Add SFX of items resource file for Item System team's requirements
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres 복사본/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/ssss/res/sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA28B87D-0B47-9D45-8CA3-8CAE03BA31D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC462CFD-D7E8-974D-A507-31EF06118DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27180" yWindow="-8560" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="74">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,6 +94,9 @@
     <t>AscendingScales2.wav</t>
   </si>
   <si>
+    <t>AscendingScales1.wav</t>
+  </si>
+  <si>
     <t>DescendingScales2.wav</t>
   </si>
   <si>
@@ -136,6 +139,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ItemGet1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>BlipLow.wav</t>
   </si>
   <si>
@@ -179,6 +186,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Audio Normalization</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -187,6 +198,38 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ShipLandingAndTakeOff.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bomb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubShip_10s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpeedUp_10s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShipTakeOff.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GreatShoot.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhoararang.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invincible_10s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>AlienSpaceship.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -244,6 +287,10 @@
   </si>
   <si>
     <t>GameplayHUD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemSystem</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -668,30 +715,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -700,13 +747,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G16" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
@@ -715,7 +762,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -724,13 +771,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -739,7 +786,7 @@
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -748,13 +795,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -763,7 +810,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -772,13 +819,13 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -787,22 +834,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -811,7 +858,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -820,13 +867,13 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -835,7 +882,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -844,13 +891,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -859,7 +906,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -868,13 +915,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -883,7 +930,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -892,13 +939,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -907,7 +954,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -916,13 +963,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -931,7 +978,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -940,13 +987,13 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -972,7 +1019,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE52464-EF18-2641-8F7C-C87CF4B5A50E}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="154" workbookViewId="0"/>
   </sheetViews>
@@ -988,30 +1035,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1020,28 +1067,28 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G20" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <f t="shared" ref="G2:G18" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
         <v>SFX_GameplayHUD_GameScreen_GameOver_DescendingScales2.wav</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1050,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -1059,22 +1106,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -1083,22 +1130,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -1107,193 +1154,313 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G6" t="str">
-        <f>_xlfn.CONCAT("SFX_",A6,"_",B6,"_",C6,"_",D6)</f>
-        <v>SFX_MainMenu_TitleScreen_MenuSelect_BlipLow.wav</v>
+        <f t="shared" si="0"/>
+        <v>SFX_ItemSystem_Item_Bomb_GreatShoot.wav</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G7" t="str">
-        <f>_xlfn.CONCAT("SFX_",A7,"_",B7,"_",C7,"_",D7)</f>
-        <v>SFX_Player&amp;EnemyShipVariety_Bullet_AllyShipShooting_LaserShootAlly1.wav</v>
+        <f t="shared" si="0"/>
+        <v>SFX_ItemSystem_Item_Invincible_10s_Zhoararang.wav</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G8" t="str">
-        <f>_xlfn.CONCAT("SFX_",A8,"_",B8,"_",C8,"_",D8)</f>
-        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipDestroy_Deleted.wav</v>
+        <f t="shared" si="0"/>
+        <v>SFX_ItemSystem_Item_ItemGet1_AscendingScales1.wav</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G9" t="str">
-        <f>_xlfn.CONCAT("SFX_",A9,"_",B9,"_",C9,"_",D9)</f>
-        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipShooting_LaserShootEnemy1.wav</v>
+        <f t="shared" si="0"/>
+        <v>SFX_ItemSystem_Item_SpeedUp_10s_ShipTakeOff.wav</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G10" t="str">
-        <f>_xlfn.CONCAT("SFX_",A10,"_",B10,"_",C10,"_",D10)</f>
-        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipSpecial_ShipAppear.wav</v>
+        <f t="shared" si="0"/>
+        <v>SFX_ItemSystem_Item_SubShip_10s_ShipLandingAndTakeOff.wav</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G11" t="str">
-        <f>_xlfn.CONCAT("SFX_",A11,"_",B11,"_",C11,"_",D11)</f>
-        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipSpecialDestroy_ExplosionShort.wav</v>
+        <f t="shared" si="0"/>
+        <v>SFX_MainMenu_TitleScreen_MenuSelect_BlipLow.wav</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
+      <c r="C12" t="s">
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G12" t="str">
-        <f>_xlfn.CONCAT("SFX_",A12,"_",B12,"_",C12,"_",D12)</f>
-        <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroy_ExplosionLong.wav</v>
+        <f t="shared" si="0"/>
+        <v>SFX_Player&amp;EnemyShipVariety_Bullet_AllyShipShooting_LaserShootAlly1.wav</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipDestroy_Deleted.wav</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipShooting_LaserShootEnemy1.wav</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipSpecial_ShipAppear.wav</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipSpecialDestroy_ExplosionShort.wav</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="G13" t="str">
-        <f>_xlfn.CONCAT("SFX_",A13,"_",B13,"_",C13,"_",D13)</f>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroy_ExplosionLong.wav</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
         <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroyLives_DescendingScales1.wav</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add SFX of achievement and score resource file for Records & Achievements System team's requirements
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/ssss/res/sound/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC462CFD-D7E8-974D-A507-31EF06118DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633015E5-A848-F346-96FD-C7663FED7A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27180" yWindow="-8560" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,12 +91,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>NewScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>AscendingScales2.wav</t>
   </si>
   <si>
     <t>AscendingScales1.wav</t>
   </si>
   <si>
+    <t>Fanfare.wav</t>
+  </si>
+  <si>
     <t>DescendingScales2.wav</t>
   </si>
   <si>
@@ -174,6 +181,10 @@
     <t>LaserShootAlly1.wav</t>
   </si>
   <si>
+    <t>ScoreScreen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Bullet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -230,6 +241,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>AchievementManager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coin.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NewAchievement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>AlienSpaceship.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -271,6 +294,10 @@
   </si>
   <si>
     <t>MainMenu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Records&amp;Achievement</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -715,30 +742,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -747,13 +774,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G16" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
@@ -762,7 +789,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -771,13 +798,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -786,7 +813,7 @@
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -795,13 +822,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -810,7 +837,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -819,13 +846,13 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -834,22 +861,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -858,7 +885,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -867,13 +894,13 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -882,7 +909,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -891,13 +918,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -906,7 +933,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -915,13 +942,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -930,7 +957,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -939,13 +966,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -954,7 +981,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -963,13 +990,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -978,7 +1005,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -987,13 +1014,13 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -1019,7 +1046,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE52464-EF18-2641-8F7C-C87CF4B5A50E}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="154" workbookViewId="0"/>
   </sheetViews>
@@ -1035,30 +1062,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1067,37 +1094,37 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G18" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <f t="shared" ref="G2:G20" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
         <v>SFX_GameplayHUD_GameScreen_GameOver_DescendingScales2.wav</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -1106,22 +1133,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -1130,22 +1157,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -1154,22 +1181,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -1178,22 +1205,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -1202,22 +1229,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -1226,22 +1253,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -1250,22 +1277,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -1274,22 +1301,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -1298,22 +1325,22 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -1322,22 +1349,22 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -1346,22 +1373,22 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -1370,22 +1397,22 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -1394,22 +1421,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
@@ -1418,22 +1445,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -1442,26 +1469,74 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroyLives_DescendingScales1.wav</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Records&amp;Achievement_AchievementManager_NewAchievement_Coin.wav</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroyLives_DescendingScales1.wav</v>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Records&amp;Achievement_ScoreScreen_NewScore_Fanfare.wav</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add BGM of achievement and score resource file for Records & Achievements System team's requirements
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/ssss/res/sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633015E5-A848-F346-96FD-C7663FED7A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87886F1C-02CB-334F-B24E-30636E6BB1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27180" yWindow="-8560" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,19 +91,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NewScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AscendingScales2.wav</t>
   </si>
   <si>
     <t>AscendingScales1.wav</t>
   </si>
   <si>
-    <t>Fanfare.wav</t>
-  </si>
-  <si>
     <t>DescendingScales2.wav</t>
   </si>
   <si>
@@ -181,175 +174,186 @@
     <t>LaserShootAlly1.wav</t>
   </si>
   <si>
+    <t>Bullet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyShip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Audio Normalization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShipLandingAndTakeOff.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bomb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubShip_10s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpeedUp_10s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShipTakeOff.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GreatShoot.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhoararang.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invincible_10s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AlienSpaceship.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceHanger.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AmbientSpace.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceInvadersOST_Earth.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceInvadersOST_Venus.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceInvaders OST_Saturn.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceInvadersOST_Uranus.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceInvadersOST_Neptune.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceInvadersOST_Pluto.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LevelDesign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainMenu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player&amp;EnemyShipVariety</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllyShipDestroyLives</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameplayHUD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemSystem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShipAppear.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceInvadersOST_Jupiter.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spacedrone.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Team</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Situation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Records&amp;Achievement</t>
+  </si>
+  <si>
+    <t>AchievementScreen</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
     <t>ScoreScreen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bullet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EnemyShip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ship</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Audio Normalization</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShipLandingAndTakeOff.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bomb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SubShip_10s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpeedUp_10s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShipTakeOff.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GreatShoot.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zhoararang.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Invincible_10s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AchievementManager</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coin.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NewAchievement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AlienSpaceship.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpaceHanger.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AmbientSpace.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpaceInvadersOST_Earth.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpaceInvadersOST_Venus.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpaceInvaders OST_Saturn.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpaceInvadersOST_Uranus.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpaceInvadersOST_Neptune.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpaceInvadersOST_Pluto.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LevelDesign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MainMenu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Records&amp;Achievement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Player&amp;EnemyShipVariety</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Level5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AllyShipDestroyLives</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameplayHUD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemSystem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShipAppear.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpaceInvadersOST_Jupiter.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spacedrone.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Team</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Class</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Situation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FileName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source</t>
+  </si>
+  <si>
+    <t>GameOver</t>
+  </si>
+  <si>
+    <t>UfoLanding.wav</t>
+  </si>
+  <si>
+    <t>HighScoreScreen</t>
+  </si>
+  <si>
+    <t>UfoSounds.wav</t>
+  </si>
+  <si>
+    <t>MorseCode.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -742,30 +746,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -774,22 +778,22 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G16" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <f t="shared" ref="G2:G12" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
         <v>BGM_LevelDesign_GameScreen_Level1_SpaceInvadersOST_Venus.wav</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -798,13 +802,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -813,7 +817,7 @@
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -822,13 +826,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -837,7 +841,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -846,13 +850,13 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -861,22 +865,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -885,7 +889,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -894,13 +898,13 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -909,7 +913,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -918,13 +922,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -933,7 +937,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -942,13 +946,13 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -957,7 +961,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -966,13 +970,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -981,7 +985,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -990,13 +994,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -1005,7 +1009,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -1014,13 +1018,13 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -1046,7 +1050,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE52464-EF18-2641-8F7C-C87CF4B5A50E}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="154" workbookViewId="0"/>
   </sheetViews>
@@ -1062,30 +1066,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1094,37 +1098,37 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G20" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <f t="shared" ref="G2:G21" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
         <v>SFX_GameplayHUD_GameScreen_GameOver_DescendingScales2.wav</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
@@ -1133,22 +1137,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -1157,22 +1161,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -1181,22 +1185,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -1205,22 +1209,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -1229,22 +1233,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -1253,22 +1257,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -1277,22 +1281,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -1301,22 +1305,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -1325,22 +1329,22 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -1349,22 +1353,22 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -1373,22 +1377,22 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -1397,22 +1401,22 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -1421,22 +1425,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
@@ -1445,22 +1449,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -1469,22 +1473,22 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
@@ -1493,50 +1497,74 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>SFX_Records&amp;Achievement_AchievementManager_NewAchievement_Coin.wav</v>
+        <v>SFX_Records&amp;Achievement_AchievementScreen_AchievementScreen_MorseCode.wav</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>SFX_Records&amp;Achievement_ScoreScreen_NewScore_Fanfare.wav</v>
+        <v>SFX_Records&amp;Achievement_ScoreScreen_GameOver_UfoLanding.wav</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>SFX_Records&amp;Achievement_HighScoreScreen_HighScoreScreen_UfoSounds.wav</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add BGM of ship moving resource file for Player & Enemy Ship Variety team's requirements
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94486FAA-56E0-C143-802B-34C3903A8C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C5E58F-D816-DD46-B98C-5C35938A6F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31960" yWindow="-8300" windowWidth="19200" windowHeight="21100" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
+    <workbookView xWindow="-31960" yWindow="-8560" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
   <sheets>
     <sheet name="BGM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="95">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -382,6 +382,18 @@
   <si>
     <t>MorseCode.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player&amp;EnemyShipVariety</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>ShipMoving</t>
+  </si>
+  <si>
+    <t>ShipMoving.wav</t>
   </si>
 </sst>
 </file>
@@ -756,9 +768,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AD9B3-E95F-7D4D-82EC-7C2F601D1C79}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="220" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -814,7 +826,7 @@
         <v>44</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G15" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
+        <f t="shared" ref="G2:G12" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
         <v>BGM_LevelDesign_GameScreen_Level1_SpaceInvadersOST_Venus.wav</v>
       </c>
     </row>
@@ -1059,51 +1071,50 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
+      <c r="G14" t="str">
+        <f>_xlfn.CONCAT("BGM_",A14,"_",B14,"_",C14,"_",D14)</f>
         <v>BGM_Records&amp;Achievement_AchievementScreen_AchievementScreen_MorseCode.wav</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_Records&amp;Achievement_ScoreScreen_GameOver_UfoLanding.wav</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1111,13 +1122,13 @@
         <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
         <v>83</v>
@@ -1126,7 +1137,31 @@
         <v>84</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("BGM_",A15,"_",B15,"_",C15,"_",D15)</f>
+        <v>BGM_Records&amp;Achievement_ScoreScreen_GameOver_UfoLanding.wav</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" t="str">
+        <f>_xlfn.CONCAT("BGM_",A16,"_",B16,"_",C16,"_",D16)</f>
         <v>BGM_Records&amp;Achievement_HighScoreScreen_HighScoreScreen_UfoSounds.wav</v>
       </c>
     </row>
@@ -1143,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE52464-EF18-2641-8F7C-C87CF4B5A50E}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="154" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="154" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>

</xml_diff>

<commit_message>
chore: Rename Sound Resources shorter
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C5E58F-D816-DD46-B98C-5C35938A6F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DE115C-0DFB-2E42-85A5-A73CDF1B3D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31960" yWindow="-8560" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="24700" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
   <sheets>
     <sheet name="BGM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="129">
   <si>
     <t>Single / Multiple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -273,10 +273,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SpaceInvaders OST_Saturn.wav</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SpaceInvadersOST_Uranus.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -394,6 +390,118 @@
   </si>
   <si>
     <t>ShipMoving.wav</t>
+  </si>
+  <si>
+    <t>B_Level1.wav</t>
+  </si>
+  <si>
+    <t>B_Level2.wav</t>
+  </si>
+  <si>
+    <t>B_Level3.wav</t>
+  </si>
+  <si>
+    <t>B_Level4.wav</t>
+  </si>
+  <si>
+    <t>B_Level5.wav</t>
+  </si>
+  <si>
+    <t>B_Level6.wav</t>
+  </si>
+  <si>
+    <t>B_Level7.wav</t>
+  </si>
+  <si>
+    <t>SpaceInvadersOST_Saturn.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B_Main_a.wav</t>
+  </si>
+  <si>
+    <t>B_Main_b.wav</t>
+  </si>
+  <si>
+    <t>B_Main_c.wav</t>
+  </si>
+  <si>
+    <t>B_Main_d.wav</t>
+  </si>
+  <si>
+    <t>B_Ship.wav</t>
+  </si>
+  <si>
+    <t>B_HighScore.wav</t>
+  </si>
+  <si>
+    <t>S_GameOver.wav</t>
+  </si>
+  <si>
+    <t>S_LevelClear.wav</t>
+  </si>
+  <si>
+    <t>S_Item_Bomb.wav</t>
+  </si>
+  <si>
+    <t>S_Item_Invicible.wav</t>
+  </si>
+  <si>
+    <t>S_Item_Get.wav</t>
+  </si>
+  <si>
+    <t>S_Item_SpeedUp.wav</t>
+  </si>
+  <si>
+    <t>S_Item_SubShip.wav</t>
+  </si>
+  <si>
+    <t>S_Enemy_Destroy_a.wav</t>
+  </si>
+  <si>
+    <t>S_Enemy_Shoot.wav</t>
+  </si>
+  <si>
+    <t>S_Enemy_Special.wav</t>
+  </si>
+  <si>
+    <t>S_Enemy_Destroy_b.wav</t>
+  </si>
+  <si>
+    <t>S_Ally_Destroy_b.wav</t>
+  </si>
+  <si>
+    <t>S_Ally_Destroy_a.wav</t>
+  </si>
+  <si>
+    <t>S__Achievement.wav</t>
+  </si>
+  <si>
+    <t>S_NewScore.wav</t>
+  </si>
+  <si>
+    <t>S_MenuClick.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S_LevelStart_b.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S_LevelStart_a.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S_Ally_Shoot_a.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B_Achieve.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B_Gameover.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -770,7 +878,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AD9B3-E95F-7D4D-82EC-7C2F601D1C79}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="220" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -780,21 +890,21 @@
     <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -803,12 +913,12 @@
         <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -825,14 +935,13 @@
       <c r="F2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2:G12" si="0">_xlfn.CONCAT("BGM_",A2,"_",B2,"_",C2,"_",D2)</f>
-        <v>BGM_LevelDesign_GameScreen_Level1_SpaceInvadersOST_Venus.wav</v>
+      <c r="G2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -841,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -849,14 +958,13 @@
       <c r="F3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_LevelDesign_GameScreen_Level2_SpaceInvadersOST_Uranus.wav</v>
+      <c r="G3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="19" customHeight="1">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -873,14 +981,13 @@
       <c r="F4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_LevelDesign_GameScreen_Level3_SpaceInvadersOST_Earth.wav</v>
+      <c r="G4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -889,7 +996,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -897,23 +1004,22 @@
       <c r="F5" t="s">
         <v>44</v>
       </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_LevelDesign_GameScreen_Level4_SpaceInvadersOST_Jupiter.wav</v>
+      <c r="G5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -921,14 +1027,13 @@
       <c r="F6" t="s">
         <v>44</v>
       </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_LevelDesign_GameScreen_Level5_SpaceInvadersOST_Neptune.wav</v>
+      <c r="G6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -937,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
@@ -945,14 +1050,13 @@
       <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_LevelDesign_GameScreen_Level6_SpaceInvadersOST_Pluto.wav</v>
+      <c r="G7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -961,7 +1065,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -969,14 +1073,13 @@
       <c r="F8" t="s">
         <v>44</v>
       </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_LevelDesign_GameScreen_Level7_SpaceInvaders OST_Saturn.wav</v>
+      <c r="G8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -985,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -993,14 +1096,13 @@
       <c r="F9" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_MainMenu_TitleScreen_Main_Spacedrone.wav</v>
+      <c r="G9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1017,14 +1119,13 @@
       <c r="F10" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_MainMenu_TitleScreen_Main_AlienSpaceship.wav</v>
+      <c r="G10" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1041,14 +1142,13 @@
       <c r="F11" t="s">
         <v>44</v>
       </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_MainMenu_TitleScreen_Main_SpaceHanger.wav</v>
+      <c r="G11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -1065,108 +1165,104 @@
       <c r="F12" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>BGM_MainMenu_TitleScreen_Main_AmbientSpace.wav</v>
+      <c r="G12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
         <v>91</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>92</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>93</v>
       </c>
-      <c r="D13" t="s">
-        <v>94</v>
-      </c>
       <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" t="s">
         <v>83</v>
       </c>
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" t="e">
-        <v>#N/A</v>
+      <c r="G13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" t="str">
-        <f>_xlfn.CONCAT("BGM_",A14,"_",B14,"_",C14,"_",D14)</f>
-        <v>BGM_Records&amp;Achievement_AchievementScreen_AchievementScreen_MorseCode.wav</v>
+      <c r="G14" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
         <v>85</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>86</v>
       </c>
-      <c r="D15" t="s">
-        <v>87</v>
-      </c>
       <c r="E15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" t="s">
         <v>83</v>
       </c>
-      <c r="F15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" t="str">
-        <f>_xlfn.CONCAT("BGM_",A15,"_",B15,"_",C15,"_",D15)</f>
-        <v>BGM_Records&amp;Achievement_ScoreScreen_GameOver_UfoLanding.wav</v>
+      <c r="G15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
         <v>88</v>
       </c>
-      <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" t="s">
-        <v>89</v>
-      </c>
       <c r="E16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" t="s">
         <v>83</v>
       </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" t="str">
-        <f>_xlfn.CONCAT("BGM_",A16,"_",B16,"_",C16,"_",D16)</f>
-        <v>BGM_Records&amp;Achievement_HighScoreScreen_HighScoreScreen_UfoSounds.wav</v>
+      <c r="G16" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F16">
     <sortCondition ref="A1:A16"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1187,21 +1283,21 @@
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1210,12 +1306,12 @@
         <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1232,14 +1328,13 @@
       <c r="F2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2:G20" si="0">_xlfn.CONCAT("SFX_",A2,"_",B2,"_",C2,"_",D2)</f>
-        <v>SFX_GameplayHUD_GameScreen_GameOver_DescendingScales2.wav</v>
+      <c r="G2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1256,14 +1351,13 @@
       <c r="F3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_GameplayHUD_GameScreen_LevelClear_AscendingScales2.wav</v>
+      <c r="G3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1280,14 +1374,13 @@
       <c r="F4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_GameplayHUD_GameScreen_LevelStartBeep_BlipHiLong.wav</v>
+      <c r="G4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -1304,14 +1397,13 @@
       <c r="F5" t="s">
         <v>44</v>
       </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_GameplayHUD_GameScreen_LevelStartCount_BlipHiShort.wav</v>
+      <c r="G5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -1328,14 +1420,13 @@
       <c r="F6" t="s">
         <v>44</v>
       </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_ItemSystem_Item_Bomb_GreatShoot.wav</v>
+      <c r="G6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1352,14 +1443,13 @@
       <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_ItemSystem_Item_Invincible_10s_Zhoararang.wav</v>
+      <c r="G7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1376,14 +1466,13 @@
       <c r="F8" t="s">
         <v>44</v>
       </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_ItemSystem_Item_ItemGet1_AscendingScales1.wav</v>
+      <c r="G8" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
@@ -1400,14 +1489,13 @@
       <c r="F9" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_ItemSystem_Item_SpeedUp_10s_ShipTakeOff.wav</v>
+      <c r="G9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -1424,14 +1512,13 @@
       <c r="F10" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_ItemSystem_Item_SubShip_10s_ShipLandingAndTakeOff.wav</v>
+      <c r="G10" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1448,14 +1535,13 @@
       <c r="F11" t="s">
         <v>44</v>
       </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_MainMenu_TitleScreen_MenuSelect_BlipLow.wav</v>
+      <c r="G11" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -1472,14 +1558,13 @@
       <c r="F12" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Player&amp;EnemyShipVariety_Bullet_AllyShipShooting_LaserShootAlly1.wav</v>
+      <c r="G12" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
@@ -1496,14 +1581,13 @@
       <c r="F13" t="s">
         <v>44</v>
       </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipDestroy_Deleted.wav</v>
+      <c r="G13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
@@ -1520,14 +1604,13 @@
       <c r="F14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipShooting_LaserShootEnemy1.wav</v>
+      <c r="G14" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -1536,7 +1619,7 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -1544,14 +1627,13 @@
       <c r="F15" t="s">
         <v>44</v>
       </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipSpecial_ShipAppear.wav</v>
+      <c r="G15" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
@@ -1568,14 +1650,13 @@
       <c r="F16" t="s">
         <v>44</v>
       </c>
-      <c r="G16" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Player&amp;EnemyShipVariety_EnemyShip_EnemyShipSpecialDestroy_ExplosionShort.wav</v>
+      <c r="G16" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
@@ -1592,20 +1673,19 @@
       <c r="F17" t="s">
         <v>44</v>
       </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroy_ExplosionLong.wav</v>
+      <c r="G17" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -1616,14 +1696,13 @@
       <c r="F18" t="s">
         <v>44</v>
       </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Player&amp;EnemyShipVariety_Ship_AllyShipDestroyLives_DescendingScales1.wav</v>
+      <c r="G18" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>53</v>
@@ -1640,14 +1719,13 @@
       <c r="F19" t="s">
         <v>44</v>
       </c>
-      <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Records&amp;Achievement_AchievementManager_NewAchievement_Coin.wav</v>
+      <c r="G19" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
@@ -1664,15 +1742,11 @@
       <c r="F20" t="s">
         <v>44</v>
       </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v>SFX_Records&amp;Achievement_ScoreScreen_NewScore_Fanfare.wav</v>
+      <c r="G20" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
-    <sortCondition ref="G2:G20"/>
-  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: fix a filename of SFX on list
</commit_message>
<xml_diff>
--- a/res/sound/SoundResourceList.xlsx
+++ b/res/sound/SoundResourceList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/soundres/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bigjam/Library/Mobile Documents/com~apple~CloudDocs/2023-2/Java-git/2023_/res/sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DE115C-0DFB-2E42-85A5-A73CDF1B3D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465FCD57-E7B3-C74A-B33F-1939A1C2E712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="24700" activeTab="1" xr2:uid="{59547212-C016-9040-9888-6FC51CB1C510}"/>
   </bookViews>
@@ -474,9 +474,6 @@
     <t>S_Ally_Destroy_a.wav</t>
   </si>
   <si>
-    <t>S__Achievement.wav</t>
-  </si>
-  <si>
     <t>S_NewScore.wav</t>
   </si>
   <si>
@@ -501,6 +498,10 @@
   </si>
   <si>
     <t>B_Gameover.wav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S_Achievement.wav</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1212,7 +1213,7 @@
         <v>83</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1235,7 +1236,7 @@
         <v>83</v>
       </c>
       <c r="G15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1274,7 +1275,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE52464-EF18-2641-8F7C-C87CF4B5A50E}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="154" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -1375,7 +1378,7 @@
         <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1398,7 +1401,7 @@
         <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1536,7 +1539,7 @@
         <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1559,7 +1562,7 @@
         <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1720,7 +1723,7 @@
         <v>44</v>
       </c>
       <c r="G19" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1743,7 +1746,7 @@
         <v>44</v>
       </c>
       <c r="G20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>